<commit_message>
Utah agg data update.
Utah agg data update.  Changes to water source type.
</commit_message>
<xml_diff>
--- a/Utah/AggregatedAmounts/UT_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/Utah/AggregatedAmounts/UT_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Utah\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0A1034-59AF-4B3E-8BCF-B6466DA4387B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7555CAC-2153-4556-8619-27285DA32BAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="6" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="4" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -777,11 +777,6 @@
     <t>https://water.utah.gov/</t>
   </si>
   <si>
-    <t>Groundwater,
-Surface Water,
-Groundwater, Surface Water</t>
-  </si>
-  <si>
     <t>Unspecified</t>
   </si>
   <si>
@@ -831,6 +826,11 @@
   </si>
   <si>
     <t>https://github.com/WSWCWaterDataExchange/MappingStatesDataToWaDE2.0/tree/master/Utah</t>
+  </si>
+  <si>
+    <t>Groundwater,
+Surface Water,
+Surface and Groundwater</t>
   </si>
 </sst>
 </file>
@@ -2929,7 +2929,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F7" s="85" t="s">
         <v>11</v>
@@ -3149,8 +3149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570AF19E-F26B-4187-B7FA-5CACB90F90DE}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F10" sqref="F9:F10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3253,7 +3253,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -3381,7 +3381,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F8" s="85" t="s">
         <v>11</v>
@@ -3413,7 +3413,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F9" s="85" t="s">
         <v>11</v>
@@ -3445,7 +3445,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="F10" s="85" t="s">
         <v>11</v>
@@ -3591,7 +3591,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>11</v>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>11</v>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>11</v>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>11</v>
@@ -3963,7 +3963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E07544-54C6-4298-B1F4-AA27E9BE2694}">
   <dimension ref="A1:K16431"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -4191,7 +4191,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="104" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>11</v>
@@ -4257,7 +4257,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>11</v>
@@ -4289,7 +4289,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>11</v>
@@ -4322,7 +4322,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F13" s="106" t="s">
         <v>11</v>
@@ -4384,7 +4384,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="85" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>11</v>
@@ -4828,7 +4828,7 @@
         <v>15</v>
       </c>
       <c r="E29" s="85" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>11</v>
@@ -4860,7 +4860,7 @@
         <v>15</v>
       </c>
       <c r="E30" s="85" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>11</v>
@@ -4924,7 +4924,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="85" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>11</v>
@@ -4956,7 +4956,7 @@
         <v>15</v>
       </c>
       <c r="E33" s="85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Utah aggregated data update.
</commit_message>
<xml_diff>
--- a/Utah/AggregatedAmounts/UT_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/Utah/AggregatedAmounts/UT_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Utah\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7555CAC-2153-4556-8619-27285DA32BAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B080990A-C91E-4453-A5A9-8EFDF1923B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="4" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="645" activeTab="2" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -741,11 +741,6 @@
 WaterYear</t>
   </si>
   <si>
-    <t>Consumptive Use, Irrigation;
-Withdrawal, Irrigation;
-Withdrawal, Public Supply</t>
-  </si>
-  <si>
     <t>UT_Consumptive Use,
 UT_Withdrawal Irrigation,
 UT_Withdrawal Public Supply</t>
@@ -831,6 +826,11 @@
     <t>Groundwater,
 Surface Water,
 Surface and Groundwater</t>
+  </si>
+  <si>
+    <t>Consumptive Use Irrigation;
+Withdrawal Irrigation;
+Withdrawal Public Supply</t>
   </si>
 </sst>
 </file>
@@ -2312,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5623B452-6320-41F9-A4C3-771E435FA050}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2410,7 +2410,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F4" s="46" t="s">
         <v>11</v>
@@ -2666,7 +2666,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="103" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F12" s="26" t="s">
         <v>11</v>
@@ -2698,7 +2698,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>11</v>
@@ -2833,7 +2833,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -2865,7 +2865,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="96" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F5" s="85" t="s">
         <v>11</v>
@@ -2897,7 +2897,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="94" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F6" s="85" t="s">
         <v>11</v>
@@ -2929,7 +2929,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="85" t="s">
         <v>11</v>
@@ -2961,7 +2961,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="105" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F8" s="85" t="s">
         <v>11</v>
@@ -2993,7 +2993,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F9" s="85" t="s">
         <v>11</v>
@@ -3025,7 +3025,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="94" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F10" s="85" t="s">
         <v>11</v>
@@ -3057,7 +3057,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F11" s="85" t="s">
         <v>11</v>
@@ -3149,7 +3149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570AF19E-F26B-4187-B7FA-5CACB90F90DE}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -3253,7 +3253,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -3381,7 +3381,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F8" s="85" t="s">
         <v>11</v>
@@ -3413,7 +3413,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F9" s="85" t="s">
         <v>11</v>
@@ -3445,7 +3445,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F10" s="85" t="s">
         <v>11</v>
@@ -3591,7 +3591,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>11</v>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>11</v>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>11</v>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>11</v>
@@ -4191,7 +4191,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="104" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>11</v>
@@ -4224,7 +4224,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="103" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>11</v>
@@ -4257,7 +4257,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>11</v>
@@ -4289,7 +4289,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>11</v>
@@ -4322,7 +4322,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F13" s="106" t="s">
         <v>11</v>
@@ -4384,7 +4384,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="85" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>11</v>
@@ -4828,7 +4828,7 @@
         <v>15</v>
       </c>
       <c r="E29" s="85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>11</v>
@@ -4860,7 +4860,7 @@
         <v>15</v>
       </c>
       <c r="E30" s="85" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>11</v>
@@ -4924,7 +4924,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="85" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>11</v>
@@ -4956,7 +4956,7 @@
         <v>15</v>
       </c>
       <c r="E33" s="85" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>11</v>

</xml_diff>